<commit_message>
Add Task break down with assignment Add Draft version of Test Template v1.0
</commit_message>
<xml_diff>
--- a/PCB/02 Plans & Actuals/2.2_WBS & Sprint plan/Task break-down_sprint(1).xlsx
+++ b/PCB/02 Plans & Actuals/2.2_WBS & Sprint plan/Task break-down_sprint(1).xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26207"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chenyang/Documents/University of Auckland/SOFTENG 761/Project Folder/761_VEL/PCB/02 Plans &amp; Actuals/2.2_WBS &amp; Sprint plan/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14680" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="19780" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 1" sheetId="1" r:id="rId1"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="70">
   <si>
     <t>DB</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -97,108 +102,180 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>5.1.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Add page</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.2.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Edit page</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.3.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>List page</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.3.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.3.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.4.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Unit Test</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.4.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Unit Test</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.5.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6.1.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Login Page</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6.2.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6.3.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.3.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.4.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Test case (Nunit &amp; Case)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Draft version (main page + team profile + Faq)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Estimation (hr)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Totally 100 hrs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Test case (Case)</t>
+  </si>
+  <si>
+    <t>Success stories list (Individual  version)</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
     <t>Dynamic page (aspx, using DB data)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>5.1.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Add page</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>5.2.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Edit page</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>5.3.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>List page</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3.3.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4.3.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4.4.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Unit Test</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>5.4.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Unit Test</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>5.5.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>6.1.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Login Page</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>6.2.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>6.3.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Prepare dammy data (All the data we need)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2.3.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3.4.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Success stories list (Individual &amp; Company version)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Test case (Nunit &amp; Case)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Draft version (main page + team profile + Faq)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Estimation (hr)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Totally 100 hrs</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>Prepare dummy data (All the data we need)</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>127</t>
+  </si>
+  <si>
+    <t>Clay</t>
+  </si>
+  <si>
+    <t>Shawn</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>Likai</t>
+  </si>
+  <si>
+    <t>Kaii</t>
+  </si>
+  <si>
+    <t>Miranda</t>
+  </si>
+  <si>
+    <t>Irene</t>
+  </si>
+  <si>
+    <t>Lulu</t>
   </si>
 </sst>
 </file>
@@ -209,14 +286,14 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -225,7 +302,7 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -234,13 +311,13 @@
       <u/>
       <sz val="12"/>
       <color theme="11"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -250,6 +327,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -290,39 +373,46 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="25">
-    <cellStyle name="普通" xfId="0" builtinId="0"/>
-    <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -648,250 +738,738 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:AE33"/>
+  <dimension ref="B1:AG33"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="AE7" sqref="AE7"/>
-    </sheetView>
+    <sheetView tabSelected="1" showRuler="0" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="220" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="2.6640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="2.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2.6640625" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="2.6640625" style="1"/>
+    <col min="2" max="26" width="2.6640625" style="1"/>
+    <col min="27" max="27" width="3.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="16384" width="2.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:31">
+    <row r="1" spans="2:33" x14ac:dyDescent="0.2">
       <c r="X1" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2" spans="2:31">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B2" s="1">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="2:31">
-      <c r="C3" s="1" t="s">
+      <c r="AG2" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="2:33" x14ac:dyDescent="0.2">
+      <c r="C3" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="2:31">
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="W3" s="2"/>
+      <c r="X3" s="2"/>
+      <c r="Y3" s="2"/>
+      <c r="Z3" s="2"/>
+      <c r="AA3" s="2"/>
+      <c r="AC3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AE3" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="2:33" x14ac:dyDescent="0.2">
       <c r="C4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="2:31">
+        <v>57</v>
+      </c>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="U4" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="V4" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="W4" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="X4" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y4" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z4" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="AA4" s="2">
+        <v>7</v>
+      </c>
+      <c r="AC4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AE4" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="2:33" x14ac:dyDescent="0.2">
+      <c r="R5" s="2"/>
+      <c r="S5" s="2"/>
+      <c r="T5" s="2"/>
+      <c r="U5" s="2"/>
+      <c r="V5" s="2"/>
+      <c r="W5" s="2"/>
+      <c r="X5" s="2"/>
+      <c r="Y5" s="2"/>
+      <c r="Z5" s="2"/>
+      <c r="AA5" s="2"/>
+    </row>
+    <row r="6" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B6" s="1">
         <v>2</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="2:31">
-      <c r="C7" s="1" t="s">
+      <c r="R6" s="2"/>
+      <c r="S6" s="2"/>
+      <c r="T6" s="2"/>
+      <c r="U6" s="2"/>
+      <c r="V6" s="2"/>
+      <c r="W6" s="2"/>
+      <c r="X6" s="2"/>
+      <c r="Y6" s="2"/>
+      <c r="Z6" s="2"/>
+      <c r="AA6" s="2"/>
+    </row>
+    <row r="7" spans="2:33" x14ac:dyDescent="0.2">
+      <c r="C7" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="2:31">
-      <c r="C8" s="1" t="s">
+      <c r="R7" s="2"/>
+      <c r="S7" s="2"/>
+      <c r="T7" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="U7" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="V7" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="W7" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="X7" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y7" s="2"/>
+      <c r="Z7" s="2"/>
+      <c r="AA7" s="2"/>
+      <c r="AD7" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="2:33" x14ac:dyDescent="0.2">
+      <c r="C8" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="2:31">
-      <c r="C9" s="1" t="s">
-        <v>38</v>
+      <c r="R8" s="2"/>
+      <c r="S8" s="2"/>
+      <c r="T8" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="U8" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="V8" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="W8" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="X8" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y8" s="2"/>
+      <c r="Z8" s="2"/>
+      <c r="AA8" s="2"/>
+      <c r="AD8" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="2:33" x14ac:dyDescent="0.2">
+      <c r="C9" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="2:31">
+      <c r="R9" s="2"/>
+      <c r="S9" s="2"/>
+      <c r="T9" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="U9" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="V9" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="W9" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="X9" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y9" s="2"/>
+      <c r="Z9" s="2"/>
+      <c r="AA9" s="2">
+        <v>25</v>
+      </c>
+      <c r="AD9" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="2:33" x14ac:dyDescent="0.2">
+      <c r="R10" s="2"/>
+      <c r="S10" s="2"/>
+      <c r="T10" s="2"/>
+      <c r="U10" s="2"/>
+      <c r="V10" s="2"/>
+      <c r="W10" s="2"/>
+      <c r="X10" s="2"/>
+      <c r="Y10" s="2"/>
+      <c r="Z10" s="2"/>
+      <c r="AA10" s="2"/>
+    </row>
+    <row r="11" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B11" s="1">
         <v>3</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="2:31">
-      <c r="C12" s="1" t="s">
+      <c r="R11" s="2"/>
+      <c r="S11" s="2"/>
+      <c r="T11" s="2"/>
+      <c r="U11" s="2"/>
+      <c r="V11" s="2"/>
+      <c r="W11" s="2"/>
+      <c r="X11" s="2"/>
+      <c r="Y11" s="2"/>
+      <c r="Z11" s="2"/>
+      <c r="AA11" s="2"/>
+    </row>
+    <row r="12" spans="2:33" x14ac:dyDescent="0.2">
+      <c r="C12" s="3" t="s">
         <v>13</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="13" spans="2:31">
+        <v>39</v>
+      </c>
+      <c r="R12" s="2"/>
+      <c r="S12" s="2"/>
+      <c r="T12" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="U12" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="V12" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="W12" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="X12" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y12" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z12" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA12" s="2"/>
+      <c r="AC12" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="2:33" x14ac:dyDescent="0.2">
       <c r="C13" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="14" spans="2:31">
+      <c r="R13" s="2"/>
+      <c r="S13" s="2"/>
+      <c r="T13" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="U13" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="V13" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="W13" s="2"/>
+      <c r="X13" s="2"/>
+      <c r="Y13" s="2"/>
+      <c r="Z13" s="2"/>
+      <c r="AA13" s="2"/>
+    </row>
+    <row r="14" spans="2:33" x14ac:dyDescent="0.2">
       <c r="C14" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="15" spans="2:31">
+        <v>42</v>
+      </c>
+      <c r="R14" s="2"/>
+      <c r="S14" s="2"/>
+      <c r="T14" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="U14" s="2"/>
+      <c r="V14" s="2"/>
+      <c r="W14" s="2"/>
+      <c r="X14" s="2"/>
+      <c r="Y14" s="2"/>
+      <c r="Z14" s="2"/>
+      <c r="AA14" s="2"/>
+    </row>
+    <row r="15" spans="2:33" x14ac:dyDescent="0.2">
       <c r="C15" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5">
+        <v>28</v>
+      </c>
+      <c r="R15" s="2"/>
+      <c r="S15" s="2"/>
+      <c r="T15" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="U15" s="2"/>
+      <c r="V15" s="2"/>
+      <c r="W15" s="2"/>
+      <c r="X15" s="2"/>
+      <c r="Y15" s="2"/>
+      <c r="Z15" s="2"/>
+      <c r="AA15" s="2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="2:33" x14ac:dyDescent="0.2">
+      <c r="R16" s="2"/>
+      <c r="S16" s="2"/>
+      <c r="T16" s="2"/>
+      <c r="U16" s="2"/>
+      <c r="V16" s="2"/>
+      <c r="W16" s="2"/>
+      <c r="X16" s="2"/>
+      <c r="Y16" s="2"/>
+      <c r="Z16" s="2"/>
+      <c r="AA16" s="2"/>
+    </row>
+    <row r="17" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B17" s="1">
         <v>4</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5">
-      <c r="C18" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R17" s="2"/>
+      <c r="S17" s="2"/>
+      <c r="T17" s="2"/>
+      <c r="U17" s="2"/>
+      <c r="V17" s="2"/>
+      <c r="W17" s="2"/>
+      <c r="X17" s="2"/>
+      <c r="Y17" s="2"/>
+      <c r="Z17" s="2"/>
+      <c r="AA17" s="2"/>
+    </row>
+    <row r="18" spans="2:29" x14ac:dyDescent="0.2">
+      <c r="C18" s="3" t="s">
         <v>16</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="19" spans="2:5">
+      <c r="R18" s="2"/>
+      <c r="S18" s="2"/>
+      <c r="T18" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="U18" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="V18" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="W18" s="2"/>
+      <c r="X18" s="2"/>
+      <c r="Y18" s="2"/>
+      <c r="Z18" s="2"/>
+      <c r="AA18" s="2"/>
+      <c r="AC18" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="2:29" x14ac:dyDescent="0.2">
       <c r="C19" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5">
+        <v>55</v>
+      </c>
+      <c r="R19" s="2"/>
+      <c r="S19" s="2"/>
+      <c r="T19" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="U19" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="V19" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="W19" s="2"/>
+      <c r="X19" s="2"/>
+      <c r="Y19" s="2"/>
+      <c r="Z19" s="2"/>
+      <c r="AA19" s="2"/>
+    </row>
+    <row r="20" spans="2:29" x14ac:dyDescent="0.2">
       <c r="C20" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="R20" s="2"/>
+      <c r="S20" s="2"/>
+      <c r="T20" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="U20" s="2"/>
+      <c r="V20" s="2"/>
+      <c r="W20" s="2"/>
+      <c r="X20" s="2"/>
+      <c r="Y20" s="2"/>
+      <c r="Z20" s="2"/>
+      <c r="AA20" s="2"/>
+      <c r="AC20" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="2:29" x14ac:dyDescent="0.2">
+      <c r="C21" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E20" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5">
-      <c r="C21" s="1" t="s">
+      <c r="E21" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E21" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5">
+      <c r="R21" s="2"/>
+      <c r="S21" s="2"/>
+      <c r="T21" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="U21" s="2"/>
+      <c r="V21" s="2"/>
+      <c r="W21" s="2"/>
+      <c r="X21" s="2"/>
+      <c r="Y21" s="2"/>
+      <c r="Z21" s="2"/>
+      <c r="AA21" s="2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="2:29" x14ac:dyDescent="0.2">
+      <c r="R22" s="2"/>
+      <c r="S22" s="2"/>
+      <c r="T22" s="2"/>
+      <c r="U22" s="2"/>
+      <c r="V22" s="2"/>
+      <c r="W22" s="2"/>
+      <c r="X22" s="2"/>
+      <c r="Y22" s="2"/>
+      <c r="Z22" s="2"/>
+      <c r="AA22" s="2"/>
+    </row>
+    <row r="23" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B23" s="1">
         <v>5</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="24" spans="2:5">
+      <c r="R23" s="2"/>
+      <c r="S23" s="2"/>
+      <c r="T23" s="2"/>
+      <c r="U23" s="2"/>
+      <c r="V23" s="2"/>
+      <c r="W23" s="2"/>
+      <c r="X23" s="2"/>
+      <c r="Y23" s="2"/>
+      <c r="Z23" s="2"/>
+      <c r="AA23" s="2"/>
+    </row>
+    <row r="24" spans="2:29" x14ac:dyDescent="0.2">
       <c r="C24" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E24" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="R24" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="S24" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="T24" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="U24" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="V24" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="W24" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="X24" s="2"/>
+      <c r="Y24" s="2"/>
+      <c r="Z24" s="2"/>
+      <c r="AA24" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="25" spans="2:29" x14ac:dyDescent="0.2">
+      <c r="C25" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="25" spans="2:5">
-      <c r="C25" s="1" t="s">
+      <c r="E25" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="R25" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="S25" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="T25" s="2"/>
+      <c r="U25" s="2"/>
+      <c r="V25" s="2"/>
+      <c r="W25" s="2"/>
+      <c r="X25" s="2"/>
+      <c r="Y25" s="2"/>
+      <c r="Z25" s="2"/>
+      <c r="AA25" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="26" spans="2:29" x14ac:dyDescent="0.2">
+      <c r="C26" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="26" spans="2:5">
-      <c r="C26" s="1" t="s">
+      <c r="E26" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E26" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27" spans="2:5">
+      <c r="R26" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="S26" s="2"/>
+      <c r="T26" s="2"/>
+      <c r="U26" s="2"/>
+      <c r="V26" s="2"/>
+      <c r="W26" s="2"/>
+      <c r="X26" s="2"/>
+      <c r="Y26" s="2"/>
+      <c r="Z26" s="2"/>
+      <c r="AA26" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="27" spans="2:29" x14ac:dyDescent="0.2">
       <c r="C27" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="R27" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="S27" s="2"/>
+      <c r="T27" s="2"/>
+      <c r="U27" s="2"/>
+      <c r="V27" s="2"/>
+      <c r="W27" s="2"/>
+      <c r="X27" s="2"/>
+      <c r="Y27" s="2"/>
+      <c r="Z27" s="2"/>
+      <c r="AA27" s="2"/>
+    </row>
+    <row r="28" spans="2:29" x14ac:dyDescent="0.2">
+      <c r="C28" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E28" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E27" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="28" spans="2:5">
-      <c r="C28" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="30" spans="2:5">
+      <c r="R28" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="S28" s="2"/>
+      <c r="T28" s="2"/>
+      <c r="U28" s="2"/>
+      <c r="V28" s="2"/>
+      <c r="W28" s="2"/>
+      <c r="X28" s="2"/>
+      <c r="Y28" s="2"/>
+      <c r="Z28" s="2"/>
+      <c r="AA28" s="2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="29" spans="2:29" x14ac:dyDescent="0.2">
+      <c r="R29" s="2"/>
+      <c r="S29" s="2"/>
+      <c r="T29" s="2"/>
+      <c r="U29" s="2"/>
+      <c r="V29" s="2"/>
+      <c r="W29" s="2"/>
+      <c r="X29" s="2"/>
+      <c r="Y29" s="2"/>
+      <c r="Z29" s="2"/>
+      <c r="AA29" s="2"/>
+    </row>
+    <row r="30" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B30" s="1">
         <v>6</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="31" spans="2:5">
+      <c r="R30" s="2"/>
+      <c r="S30" s="2"/>
+      <c r="T30" s="2"/>
+      <c r="U30" s="2"/>
+      <c r="V30" s="2"/>
+      <c r="W30" s="2"/>
+      <c r="X30" s="2"/>
+      <c r="Y30" s="2"/>
+      <c r="Z30" s="2"/>
+      <c r="AA30" s="2"/>
+    </row>
+    <row r="31" spans="2:29" x14ac:dyDescent="0.2">
       <c r="C31" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E31" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="R31" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="S31" s="2"/>
+      <c r="T31" s="2"/>
+      <c r="U31" s="2"/>
+      <c r="V31" s="2"/>
+      <c r="W31" s="2"/>
+      <c r="X31" s="2"/>
+      <c r="Y31" s="2"/>
+      <c r="Z31" s="2"/>
+      <c r="AA31" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="32" spans="2:29" x14ac:dyDescent="0.2">
+      <c r="C32" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="32" spans="2:5">
-      <c r="C32" s="1" t="s">
+      <c r="E32" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="R32" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="S32" s="2"/>
+      <c r="T32" s="2"/>
+      <c r="U32" s="2"/>
+      <c r="V32" s="2"/>
+      <c r="W32" s="2"/>
+      <c r="X32" s="2"/>
+      <c r="Y32" s="2"/>
+      <c r="Z32" s="2"/>
+      <c r="AA32" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="33" spans="3:27" x14ac:dyDescent="0.2">
+      <c r="C33" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E32" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="33" spans="3:5">
-      <c r="C33" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="E33" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
+      </c>
+      <c r="R33" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="S33" s="2"/>
+      <c r="T33" s="2"/>
+      <c r="U33" s="2"/>
+      <c r="V33" s="2"/>
+      <c r="W33" s="2"/>
+      <c r="X33" s="2"/>
+      <c r="Y33" s="2"/>
+      <c r="Z33" s="2"/>
+      <c r="AA33" s="2">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update the task with 5.4-5.6. (Kaii)
</commit_message>
<xml_diff>
--- a/PCB/02 Plans & Actuals/2.2_WBS & Sprint plan/Task break-down_sprint(1).xlsx
+++ b/PCB/02 Plans & Actuals/2.2_WBS & Sprint plan/Task break-down_sprint(1).xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26207"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chenyang/Documents/University of Auckland/SOFTENG 761/Project Folder/761_VEL/PCB/02 Plans &amp; Actuals/2.2_WBS &amp; Sprint plan/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="19780" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14680" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 1" sheetId="1" r:id="rId1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="72">
   <si>
     <t>DB</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -62,220 +57,227 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>Solution Create (with DB connect, team)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.2.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.1.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.2.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Updated version</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.1.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.2.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Statics page design (layout, mobile-friendly)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.1.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Add page</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.2.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Edit page</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.3.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>List page</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.3.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.3.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.4.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Unit Test</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.4.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Unit Test</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.5.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6.1.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Login Page</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6.2.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6.3.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.3.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.4.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Test case (Nunit &amp; Case)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Draft version (main page + team profile + Faq)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Estimation (hr)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Totally 100 hrs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Test case (Case)</t>
+  </si>
+  <si>
+    <t>Success stories list (Individual  version)</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>Dynamic page (aspx, using DB data)</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>127</t>
+  </si>
+  <si>
+    <t>Clay</t>
+  </si>
+  <si>
+    <t>Shawn</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>Likai</t>
+  </si>
+  <si>
+    <t>Kaii</t>
+  </si>
+  <si>
+    <t>Miranda</t>
+  </si>
+  <si>
+    <t>Irene</t>
+  </si>
+  <si>
+    <t>Lulu</t>
+  </si>
+  <si>
     <t>1.1.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Solution Create (with DB connect, team)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1.2.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Create New DB</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>3.1.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3.2.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Updated version</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4.1.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4.2.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Statics page design (layout, mobile-friendly)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>5.1.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Add page</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>5.2.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Edit page</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>5.3.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>List page</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3.3.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4.3.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4.4.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Unit Test</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>5.4.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Unit Test</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>5.5.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>6.1.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Login Page</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>6.2.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>6.3.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2.3.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3.4.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Test case (Nunit &amp; Case)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Draft version (main page + team profile + Faq)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Estimation (hr)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Totally 100 hrs</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Test case (Case)</t>
-  </si>
-  <si>
-    <t>Success stories list (Individual  version)</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>Dynamic page (aspx, using DB data)</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
     <t>Prepare dummy data (All the data we need)</t>
-  </si>
-  <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>127</t>
-  </si>
-  <si>
-    <t>Clay</t>
-  </si>
-  <si>
-    <t>Shawn</t>
-  </si>
-  <si>
-    <t>V</t>
-  </si>
-  <si>
-    <t>Likai</t>
-  </si>
-  <si>
-    <t>Kaii</t>
-  </si>
-  <si>
-    <t>Miranda</t>
-  </si>
-  <si>
-    <t>Irene</t>
-  </si>
-  <si>
-    <t>Lulu</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.6.</t>
+  </si>
+  <si>
+    <t>5.7.</t>
   </si>
 </sst>
 </file>
@@ -286,14 +288,14 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -302,7 +304,7 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -311,7 +313,7 @@
       <u/>
       <sz val="12"/>
       <color theme="11"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -346,8 +348,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="25">
+  <cellStyleXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -379,32 +389,40 @@
     <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="25">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="33">
+    <cellStyle name="普通" xfId="0" builtinId="0"/>
+    <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="31" builtinId="8" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -738,11 +756,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:AG33"/>
+  <dimension ref="B1:AG35"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="220" workbookViewId="0"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="U25" sqref="U25"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="2.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="2.6640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="2.6640625" style="1" customWidth="1"/>
     <col min="2" max="26" width="2.6640625" style="1"/>
@@ -750,15 +770,15 @@
     <col min="28" max="16384" width="2.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:33" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:33">
       <c r="X1" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="2" spans="2:33" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="2:33">
       <c r="B2" s="1">
         <v>1</v>
       </c>
@@ -766,26 +786,26 @@
         <v>0</v>
       </c>
       <c r="AG2" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="3" spans="2:33" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="2:33">
       <c r="C3" s="3" t="s">
-        <v>9</v>
+        <v>67</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>12</v>
+        <v>68</v>
       </c>
       <c r="R3" s="2"/>
       <c r="S3" s="2"/>
       <c r="T3" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="U3" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="V3" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
@@ -793,53 +813,53 @@
       <c r="Z3" s="2"/>
       <c r="AA3" s="2"/>
       <c r="AC3" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="AE3" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="4" spans="2:33" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="2:33">
       <c r="C4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="R4" s="2"/>
       <c r="S4" s="2"/>
       <c r="T4" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="U4" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="V4" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="W4" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="X4" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="Y4" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="Z4" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="AA4" s="2">
         <v>7</v>
       </c>
       <c r="AC4" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="AE4" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="5" spans="2:33" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="2:33">
       <c r="R5" s="2"/>
       <c r="S5" s="2"/>
       <c r="T5" s="2"/>
@@ -851,7 +871,7 @@
       <c r="Z5" s="2"/>
       <c r="AA5" s="2"/>
     </row>
-    <row r="6" spans="2:33" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:33">
       <c r="B6" s="1">
         <v>2</v>
       </c>
@@ -869,38 +889,38 @@
       <c r="Z6" s="2"/>
       <c r="AA6" s="2"/>
     </row>
-    <row r="7" spans="2:33" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:33">
       <c r="C7" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="R7" s="2"/>
       <c r="S7" s="2"/>
       <c r="T7" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="U7" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="V7" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="W7" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="X7" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="Y7" s="2"/>
       <c r="Z7" s="2"/>
       <c r="AA7" s="2"/>
       <c r="AD7" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="8" spans="2:33" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="2:33">
       <c r="C8" s="3" t="s">
         <v>6</v>
       </c>
@@ -910,30 +930,30 @@
       <c r="R8" s="2"/>
       <c r="S8" s="2"/>
       <c r="T8" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="U8" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="V8" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="W8" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="X8" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="U8" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="V8" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="W8" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="X8" s="2" t="s">
-        <v>47</v>
       </c>
       <c r="Y8" s="2"/>
       <c r="Z8" s="2"/>
       <c r="AA8" s="2"/>
       <c r="AD8" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="9" spans="2:33" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="2:33">
       <c r="C9" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>8</v>
@@ -941,19 +961,19 @@
       <c r="R9" s="2"/>
       <c r="S9" s="2"/>
       <c r="T9" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="U9" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="V9" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="W9" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="X9" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="X9" s="2" t="s">
-        <v>46</v>
       </c>
       <c r="Y9" s="2"/>
       <c r="Z9" s="2"/>
@@ -961,10 +981,10 @@
         <v>25</v>
       </c>
       <c r="AD9" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="10" spans="2:33" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="2:33">
       <c r="R10" s="2"/>
       <c r="S10" s="2"/>
       <c r="T10" s="2"/>
@@ -976,7 +996,7 @@
       <c r="Z10" s="2"/>
       <c r="AA10" s="2"/>
     </row>
-    <row r="11" spans="2:33" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:33">
       <c r="B11" s="1">
         <v>3</v>
       </c>
@@ -994,58 +1014,58 @@
       <c r="Z11" s="2"/>
       <c r="AA11" s="2"/>
     </row>
-    <row r="12" spans="2:33" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:33">
       <c r="C12" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="R12" s="2"/>
       <c r="S12" s="2"/>
       <c r="T12" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="U12" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="V12" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="W12" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="X12" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y12" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z12" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="X12" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="Y12" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="Z12" s="2" t="s">
-        <v>46</v>
       </c>
       <c r="AA12" s="2"/>
       <c r="AC12" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="13" spans="2:33" x14ac:dyDescent="0.2">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="2:33">
       <c r="C13" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="R13" s="2"/>
       <c r="S13" s="2"/>
       <c r="T13" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="U13" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="V13" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="W13" s="2"/>
       <c r="X13" s="2"/>
@@ -1053,17 +1073,17 @@
       <c r="Z13" s="2"/>
       <c r="AA13" s="2"/>
     </row>
-    <row r="14" spans="2:33" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:33">
       <c r="C14" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="R14" s="2"/>
       <c r="S14" s="2"/>
       <c r="T14" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="U14" s="2"/>
       <c r="V14" s="2"/>
@@ -1073,17 +1093,17 @@
       <c r="Z14" s="2"/>
       <c r="AA14" s="2"/>
     </row>
-    <row r="15" spans="2:33" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:33">
       <c r="C15" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="R15" s="2"/>
       <c r="S15" s="2"/>
       <c r="T15" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="U15" s="2"/>
       <c r="V15" s="2"/>
@@ -1095,7 +1115,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="2:33" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:33">
       <c r="R16" s="2"/>
       <c r="S16" s="2"/>
       <c r="T16" s="2"/>
@@ -1107,12 +1127,12 @@
       <c r="Z16" s="2"/>
       <c r="AA16" s="2"/>
     </row>
-    <row r="17" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:29">
       <c r="B17" s="1">
         <v>4</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="R17" s="2"/>
       <c r="S17" s="2"/>
@@ -1125,23 +1145,23 @@
       <c r="Z17" s="2"/>
       <c r="AA17" s="2"/>
     </row>
-    <row r="18" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:29">
       <c r="C18" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="R18" s="2"/>
       <c r="S18" s="2"/>
       <c r="T18" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="U18" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="V18" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="W18" s="2"/>
       <c r="X18" s="2"/>
@@ -1149,26 +1169,26 @@
       <c r="Z18" s="2"/>
       <c r="AA18" s="2"/>
       <c r="AC18" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="19" spans="2:29" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="2:29">
       <c r="C19" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="R19" s="2"/>
       <c r="S19" s="2"/>
       <c r="T19" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="U19" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="V19" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="W19" s="2"/>
       <c r="X19" s="2"/>
@@ -1176,17 +1196,17 @@
       <c r="Z19" s="2"/>
       <c r="AA19" s="2"/>
     </row>
-    <row r="20" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:29">
       <c r="C20" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="R20" s="2"/>
       <c r="S20" s="2"/>
       <c r="T20" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="U20" s="2"/>
       <c r="V20" s="2"/>
@@ -1196,20 +1216,20 @@
       <c r="Z20" s="2"/>
       <c r="AA20" s="2"/>
       <c r="AC20" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="21" spans="2:29" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="2:29">
       <c r="C21" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="R21" s="2"/>
       <c r="S21" s="2"/>
       <c r="T21" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="U21" s="2"/>
       <c r="V21" s="2"/>
@@ -1221,7 +1241,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:29">
       <c r="R22" s="2"/>
       <c r="S22" s="2"/>
       <c r="T22" s="2"/>
@@ -1233,7 +1253,7 @@
       <c r="Z22" s="2"/>
       <c r="AA22" s="2"/>
     </row>
-    <row r="23" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:29">
       <c r="B23" s="1">
         <v>5</v>
       </c>
@@ -1251,50 +1271,50 @@
       <c r="Z23" s="2"/>
       <c r="AA23" s="2"/>
     </row>
-    <row r="24" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:29">
       <c r="C24" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="R24" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="S24" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="T24" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="T24" s="2" t="s">
-        <v>48</v>
-      </c>
       <c r="U24" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="V24" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="W24" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="X24" s="2"/>
       <c r="Y24" s="2"/>
       <c r="Z24" s="2"/>
       <c r="AA24" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="25" spans="2:29" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="2:29">
       <c r="C25" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="R25" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="S25" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="T25" s="2"/>
       <c r="U25" s="2"/>
@@ -1304,18 +1324,18 @@
       <c r="Y25" s="2"/>
       <c r="Z25" s="2"/>
       <c r="AA25" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="26" spans="2:29" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="26" spans="2:29">
       <c r="C26" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="R26" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="S26" s="2"/>
       <c r="T26" s="2"/>
@@ -1326,18 +1346,18 @@
       <c r="Y26" s="2"/>
       <c r="Z26" s="2"/>
       <c r="AA26" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="27" spans="2:29" x14ac:dyDescent="0.2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="27" spans="2:29">
       <c r="C27" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="R27" s="2" t="s">
-        <v>51</v>
+        <v>36</v>
+      </c>
+      <c r="R27" s="2">
+        <v>4</v>
       </c>
       <c r="S27" s="2"/>
       <c r="T27" s="2"/>
@@ -1349,15 +1369,15 @@
       <c r="Z27" s="2"/>
       <c r="AA27" s="2"/>
     </row>
-    <row r="28" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:29">
       <c r="C28" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="R28" s="2" t="s">
-        <v>50</v>
+        <v>36</v>
+      </c>
+      <c r="R28" s="2">
+        <v>4</v>
       </c>
       <c r="S28" s="2"/>
       <c r="T28" s="2"/>
@@ -1367,12 +1387,18 @@
       <c r="X28" s="2"/>
       <c r="Y28" s="2"/>
       <c r="Z28" s="2"/>
-      <c r="AA28" s="2">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="29" spans="2:29" x14ac:dyDescent="0.2">
-      <c r="R29" s="2"/>
+      <c r="AA28" s="2"/>
+    </row>
+    <row r="29" spans="2:29">
+      <c r="C29" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="R29" s="2">
+        <v>4</v>
+      </c>
       <c r="S29" s="2"/>
       <c r="T29" s="2"/>
       <c r="U29" s="2"/>
@@ -1383,14 +1409,16 @@
       <c r="Z29" s="2"/>
       <c r="AA29" s="2"/>
     </row>
-    <row r="30" spans="2:29" x14ac:dyDescent="0.2">
-      <c r="B30" s="1">
-        <v>6</v>
-      </c>
+    <row r="30" spans="2:29">
       <c r="C30" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="R30" s="2"/>
+        <v>71</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="R30" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="S30" s="2"/>
       <c r="T30" s="2"/>
       <c r="U30" s="2"/>
@@ -1399,18 +1427,12 @@
       <c r="X30" s="2"/>
       <c r="Y30" s="2"/>
       <c r="Z30" s="2"/>
-      <c r="AA30" s="2"/>
-    </row>
-    <row r="31" spans="2:29" x14ac:dyDescent="0.2">
-      <c r="C31" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="R31" s="2" t="s">
-        <v>45</v>
-      </c>
+      <c r="AA30" s="2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="31" spans="2:29">
+      <c r="R31" s="2"/>
       <c r="S31" s="2"/>
       <c r="T31" s="2"/>
       <c r="U31" s="2"/>
@@ -1419,20 +1441,16 @@
       <c r="X31" s="2"/>
       <c r="Y31" s="2"/>
       <c r="Z31" s="2"/>
-      <c r="AA31" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="32" spans="2:29" x14ac:dyDescent="0.2">
+      <c r="AA31" s="2"/>
+    </row>
+    <row r="32" spans="2:29">
+      <c r="B32" s="1">
+        <v>6</v>
+      </c>
       <c r="C32" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="R32" s="2" t="s">
-        <v>47</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="R32" s="2"/>
       <c r="S32" s="2"/>
       <c r="T32" s="2"/>
       <c r="U32" s="2"/>
@@ -1441,19 +1459,17 @@
       <c r="X32" s="2"/>
       <c r="Y32" s="2"/>
       <c r="Z32" s="2"/>
-      <c r="AA32" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="33" spans="3:27" x14ac:dyDescent="0.2">
+      <c r="AA32" s="2"/>
+    </row>
+    <row r="33" spans="3:27">
       <c r="C33" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="R33" s="2" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="S33" s="2"/>
       <c r="T33" s="2"/>
@@ -1463,7 +1479,51 @@
       <c r="X33" s="2"/>
       <c r="Y33" s="2"/>
       <c r="Z33" s="2"/>
-      <c r="AA33" s="2">
+      <c r="AA33" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="34" spans="3:27">
+      <c r="C34" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="R34" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="S34" s="2"/>
+      <c r="T34" s="2"/>
+      <c r="U34" s="2"/>
+      <c r="V34" s="2"/>
+      <c r="W34" s="2"/>
+      <c r="X34" s="2"/>
+      <c r="Y34" s="2"/>
+      <c r="Z34" s="2"/>
+      <c r="AA34" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="35" spans="3:27">
+      <c r="C35" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="R35" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="S35" s="2"/>
+      <c r="T35" s="2"/>
+      <c r="U35" s="2"/>
+      <c r="V35" s="2"/>
+      <c r="W35" s="2"/>
+      <c r="X35" s="2"/>
+      <c r="Y35" s="2"/>
+      <c r="Z35" s="2"/>
+      <c r="AA35" s="2">
         <v>11</v>
       </c>
     </row>
@@ -1471,5 +1531,10 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>